<commit_message>
Added in Current day's prices to the dataframe using googlefinance API
</commit_message>
<xml_diff>
--- a/share_test.xlsx
+++ b/share_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>AAL</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>2017-08-18</t>
   </si>
 </sst>
 </file>
@@ -452,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y413"/>
+  <dimension ref="A1:Y414"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -31770,6 +31773,83 @@
         <v>0</v>
       </c>
     </row>
+    <row r="414" spans="1:25">
+      <c r="A414" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B414">
+        <v>1279</v>
+      </c>
+      <c r="C414">
+        <v>3141</v>
+      </c>
+      <c r="D414">
+        <v>440.3</v>
+      </c>
+      <c r="E414">
+        <v>521.85</v>
+      </c>
+      <c r="F414">
+        <v>1273.759617967626</v>
+      </c>
+      <c r="G414">
+        <v>3156.964561938146</v>
+      </c>
+      <c r="H414">
+        <v>471.9916409762618</v>
+      </c>
+      <c r="I414">
+        <v>497.1386054513881</v>
+      </c>
+      <c r="J414">
+        <v>1262.105296297543</v>
+      </c>
+      <c r="K414">
+        <v>3127.691707347916</v>
+      </c>
+      <c r="L414">
+        <v>462.0129033519668</v>
+      </c>
+      <c r="M414">
+        <v>514.1526699406778</v>
+      </c>
+      <c r="N414">
+        <v>1220.373837977253</v>
+      </c>
+      <c r="O414">
+        <v>3067.678906831986</v>
+      </c>
+      <c r="P414">
+        <v>457.3134430059133</v>
+      </c>
+      <c r="Q414">
+        <v>522.9974515782235</v>
+      </c>
+      <c r="R414" t="b">
+        <v>0</v>
+      </c>
+      <c r="S414" t="b">
+        <v>0</v>
+      </c>
+      <c r="T414" t="b">
+        <v>0</v>
+      </c>
+      <c r="U414" t="b">
+        <v>1</v>
+      </c>
+      <c r="V414" t="b">
+        <v>1</v>
+      </c>
+      <c r="W414" t="b">
+        <v>1</v>
+      </c>
+      <c r="X414" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y414" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed date for todays prices to enable plotting
</commit_message>
<xml_diff>
--- a/share_test.xlsx
+++ b/share_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>AAL</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>2017-08-18</t>
   </si>
 </sst>
 </file>
@@ -31774,56 +31771,56 @@
       </c>
     </row>
     <row r="414" spans="1:25">
-      <c r="A414" s="1" t="s">
-        <v>25</v>
+      <c r="A414" s="2">
+        <v>42965.73024815752</v>
       </c>
       <c r="B414">
-        <v>1279</v>
+        <v>1267.6</v>
       </c>
       <c r="C414">
-        <v>3141</v>
+        <v>3135.84</v>
       </c>
       <c r="D414">
-        <v>440.3</v>
+        <v>439.92</v>
       </c>
       <c r="E414">
-        <v>521.85</v>
+        <v>520.2</v>
       </c>
       <c r="F414">
-        <v>1273.759617967626</v>
+        <v>1269.959617967626</v>
       </c>
       <c r="G414">
-        <v>3156.964561938146</v>
+        <v>3155.244561938146</v>
       </c>
       <c r="H414">
-        <v>471.9916409762618</v>
+        <v>471.4416409762619</v>
       </c>
       <c r="I414">
-        <v>497.1386054513881</v>
+        <v>497.0119387847214</v>
       </c>
       <c r="J414">
-        <v>1262.105296297543</v>
+        <v>1260.351450143697</v>
       </c>
       <c r="K414">
-        <v>3127.691707347916</v>
+        <v>3126.89786119407</v>
       </c>
       <c r="L414">
-        <v>462.0129033519668</v>
+        <v>461.7590571981206</v>
       </c>
       <c r="M414">
-        <v>514.1526699406778</v>
+        <v>514.0942084022163</v>
       </c>
       <c r="N414">
-        <v>1220.373837977253</v>
+        <v>1219.529393532809</v>
       </c>
       <c r="O414">
-        <v>3067.678906831986</v>
+        <v>3067.296684609764</v>
       </c>
       <c r="P414">
-        <v>457.3134430059133</v>
+        <v>457.1912207836911</v>
       </c>
       <c r="Q414">
-        <v>522.9974515782235</v>
+        <v>522.9693034300753</v>
       </c>
       <c r="R414" t="b">
         <v>0</v>

</xml_diff>